<commit_message>
nearly done with sample data
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9998AA35-9449-C145-AC98-5FA3CBA61D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF61EF-4D72-AF4A-9378-EB22C70B84E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -162,13 +162,124 @@
   </si>
   <si>
     <t>PRICE</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Galaxy</t>
+  </si>
+  <si>
+    <t>Icelandic Premier League</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Melbourne City FC</t>
+  </si>
+  <si>
+    <t>GoalKeeper</t>
+  </si>
+  <si>
+    <t>Striker</t>
+  </si>
+  <si>
+    <t>Midfielder</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Janitor</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Equipment Manager</t>
+  </si>
+  <si>
+    <t>Bus Driver</t>
+  </si>
+  <si>
+    <t>Wembly</t>
+  </si>
+  <si>
+    <t>Azteca</t>
+  </si>
+  <si>
+    <t>Stamford</t>
+  </si>
+  <si>
+    <t>Celtic</t>
+  </si>
+  <si>
+    <t>Emirates</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>John Johnson</t>
+  </si>
+  <si>
+    <t>johnSmith@gmail.com</t>
+  </si>
+  <si>
+    <t>janeSmith@gmail.com</t>
+  </si>
+  <si>
+    <t>johnDoe@gmail.com</t>
+  </si>
+  <si>
+    <t>janeDoe@gmail.com</t>
+  </si>
+  <si>
+    <t>johnJohnson@gmail.com</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Semi-Final</t>
+  </si>
+  <si>
+    <t>Quarter-Final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,6 +297,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,22 +343,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,13 +674,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -570,9 +707,6 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -596,67 +730,121 @@
       <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2">
+        <v>310000000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H3" s="2">
+        <v>82180</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2">
+        <v>372295</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2014</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2014</v>
+      </c>
+      <c r="H4" s="2">
+        <v>42859</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2">
+        <v>55000000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2010</v>
+      </c>
+      <c r="H5" s="2">
+        <v>62098</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2">
+        <v>83000000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2006</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2006</v>
+      </c>
+      <c r="H6" s="2">
+        <v>55608</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2">
+        <v>25000000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2002</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H7" s="2">
+        <v>78242</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -705,64 +893,164 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1586</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6420</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2002</v>
+      </c>
+      <c r="L11" s="2">
+        <v>78242</v>
+      </c>
+      <c r="M11" s="2">
+        <v>6420</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2741</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6620</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2014</v>
+      </c>
+      <c r="L12" s="2">
+        <v>42859</v>
+      </c>
+      <c r="M12" s="2">
+        <v>6620</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4443</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5561</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2002</v>
+      </c>
+      <c r="L13" s="2">
+        <v>78242</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5561</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4047</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5991</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2014</v>
+      </c>
+      <c r="L14" s="2">
+        <v>42859</v>
+      </c>
+      <c r="M14" s="2">
+        <v>5991</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2">
+        <v>8968</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3292</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2010</v>
+      </c>
+      <c r="L15" s="2">
+        <v>62098</v>
+      </c>
+      <c r="M15" s="2">
+        <v>3292</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -817,233 +1105,701 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2">
+        <v>897449</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F19" s="2">
+        <v>82180</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H19" s="2">
+        <v>78242</v>
+      </c>
+      <c r="J19" s="2">
+        <v>962067</v>
+      </c>
+      <c r="L19" s="2">
+        <v>897449</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2">
+        <v>876960</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F20" s="2">
+        <v>42859</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2006</v>
+      </c>
+      <c r="H20" s="2">
+        <v>55608</v>
+      </c>
+      <c r="J20" s="2">
+        <v>635287</v>
+      </c>
+      <c r="L20" s="2">
+        <v>876960</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N20" s="2">
+        <v>2</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2">
+        <v>755050</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2010</v>
+      </c>
+      <c r="F21" s="2">
+        <v>62098</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H21" s="2">
+        <v>82180</v>
+      </c>
+      <c r="J21" s="2">
+        <v>619043</v>
+      </c>
+      <c r="L21" s="2">
+        <v>755050</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N21" s="2">
+        <v>2</v>
+      </c>
+      <c r="O21" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2">
+        <v>707650</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2006</v>
+      </c>
+      <c r="F22" s="2">
+        <v>55608</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2014</v>
+      </c>
+      <c r="H22" s="2">
+        <v>42859</v>
+      </c>
+      <c r="J22" s="2">
+        <v>849739</v>
+      </c>
+      <c r="L22" s="2">
+        <v>707650</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2">
+        <v>364820</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2002</v>
+      </c>
+      <c r="F23" s="2">
+        <v>78242</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2010</v>
+      </c>
+      <c r="H23" s="2">
+        <v>62098</v>
+      </c>
+      <c r="J23" s="2">
+        <v>228564</v>
+      </c>
+      <c r="L23" s="2">
+        <v>364820</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>962067</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F24" s="2">
+        <v>82180</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="A25" s="2">
+        <v>635287</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2014</v>
+      </c>
+      <c r="F25" s="2">
+        <v>42859</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A26" s="2">
+        <v>619043</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2010</v>
+      </c>
+      <c r="F26" s="2">
+        <v>62098</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2">
+        <v>849739</v>
+      </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2006</v>
+      </c>
+      <c r="F27" s="2">
+        <v>55608</v>
+      </c>
       <c r="G27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2">
+        <v>228564</v>
+      </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2002</v>
+      </c>
+      <c r="F28" s="2">
+        <v>78242</v>
+      </c>
       <c r="G28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="A30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>6420</v>
+      </c>
+      <c r="B32" s="2">
+        <v>635287</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>6420</v>
+      </c>
+      <c r="F32" s="2">
+        <v>635287</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
+      <c r="I32" s="2">
+        <v>918</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>6620</v>
+      </c>
+      <c r="B33" s="2">
+        <v>228564</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>6620</v>
+      </c>
+      <c r="F33" s="2">
+        <v>228564</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>501</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>5561</v>
+      </c>
+      <c r="B34" s="2">
+        <v>897449</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>5561</v>
+      </c>
+      <c r="F34" s="2">
+        <v>897449</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+      <c r="I34" s="2">
+        <v>168</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>5991</v>
+      </c>
+      <c r="B35" s="2">
+        <v>876960</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>5991</v>
+      </c>
+      <c r="F35" s="2">
+        <v>876960</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2</v>
+      </c>
+      <c r="I35" s="2">
+        <v>576</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>3292</v>
+      </c>
+      <c r="B36" s="2">
+        <v>755050</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3292</v>
+      </c>
+      <c r="F36" s="2">
+        <v>755050</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>804</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2">
+        <v>707650</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2">
+        <v>707650</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2">
+        <v>364820</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2">
+        <v>364820</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2">
+        <v>962067</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2">
+        <v>962067</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2">
+        <v>619043</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2">
+        <v>619043</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2">
+        <v>849739</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2">
+        <v>849739</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="F44" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>897449</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2">
+        <v>918</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="F45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>876960</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2">
+        <v>501</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="F46" s="2">
+        <v>6420</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>755050</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2">
+        <v>168</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="F47" s="2">
+        <v>6620</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>707650</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2">
+        <v>576</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="F48" s="2">
+        <v>5561</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>364820</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2">
+        <v>804</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="F49" s="2">
+        <v>5991</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F50" s="2">
+        <v>3292</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F51" s="2">
+        <v>1586</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F52" s="2">
+        <v>2741</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F53" s="2">
+        <v>4443</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F54" s="2">
+        <v>4047</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F55" s="2">
+        <v>8968</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K32" r:id="rId1" xr:uid="{8D2938E3-2C74-BE45-AED8-8AB6B196051E}"/>
+    <hyperlink ref="K33" r:id="rId2" xr:uid="{BBD6F168-A99E-A445-AA2C-BAA418DFB6E6}"/>
+    <hyperlink ref="K34" r:id="rId3" xr:uid="{DF7ACF3A-6AAE-EB47-B3ED-1DE41982F532}"/>
+    <hyperlink ref="K35" r:id="rId4" xr:uid="{B7D456BD-220D-AE41-AC76-5DB386CBCFA7}"/>
+    <hyperlink ref="K36" r:id="rId5" xr:uid="{7C1C7E9F-593E-D349-9489-DC2EA7F0DA6F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i think we have rectified all match and player data
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18209F5-310F-F44E-A00D-B92DC85107B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0654F1BA-3710-6942-A7D1-8A92DB8D2A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="500" windowWidth="55800" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -176,6 +176,9 @@
     <t>Australia</t>
   </si>
   <si>
+    <t>iceland</t>
+  </si>
+  <si>
     <t>Iceland</t>
   </si>
   <si>
@@ -273,13 +276,82 @@
   </si>
   <si>
     <t>Quarter-Final</t>
+  </si>
+  <si>
+    <t>all england</t>
+  </si>
+  <si>
+    <t>united states</t>
+  </si>
+  <si>
+    <t>england+iceland</t>
+  </si>
+  <si>
+    <t>england+united states</t>
+  </si>
+  <si>
+    <t>england+australia</t>
+  </si>
+  <si>
+    <t>england+germany</t>
+  </si>
+  <si>
+    <t>australian</t>
+  </si>
+  <si>
+    <t>australia+germany 2018</t>
+  </si>
+  <si>
+    <t>united states+germany 2018</t>
+  </si>
+  <si>
+    <t>united states+england 2018</t>
+  </si>
+  <si>
+    <t>united states+australia 2018</t>
+  </si>
+  <si>
+    <t>australia+england 2018</t>
+  </si>
+  <si>
+    <t>table has more connections^^^</t>
+  </si>
+  <si>
+    <t>england+united states 2014</t>
+  </si>
+  <si>
+    <t>england+iceland 2018</t>
+  </si>
+  <si>
+    <t>england+australia 2010</t>
+  </si>
+  <si>
+    <t>england+germany 2006</t>
+  </si>
+  <si>
+    <t>england+iceland 2002</t>
+  </si>
+  <si>
+    <t>england 2018</t>
+  </si>
+  <si>
+    <t>england 2002</t>
+  </si>
+  <si>
+    <t>england 2014</t>
+  </si>
+  <si>
+    <t>england 2010</t>
+  </si>
+  <si>
+    <t>england 2006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -302,6 +374,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -309,8 +388,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +419,23 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -343,25 +446,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="6" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -674,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,11 +795,12 @@
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+    <col min="9" max="9" width="28.83203125" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
@@ -758,10 +869,10 @@
         <v>918</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>42</v>
@@ -773,7 +884,7 @@
         <v>897449</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M3" s="2">
         <v>1</v>
@@ -784,7 +895,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2">
         <v>372295</v>
@@ -793,13 +904,13 @@
         <v>501</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I4" s="2">
         <v>635287</v>
@@ -808,7 +919,7 @@
         <v>876960</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
@@ -828,10 +939,10 @@
         <v>168</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>43</v>
@@ -843,7 +954,7 @@
         <v>755050</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M5" s="2">
         <v>2</v>
@@ -863,10 +974,10 @@
         <v>576</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>44</v>
@@ -878,7 +989,7 @@
         <v>707650</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M6" s="2">
         <v>0</v>
@@ -898,10 +1009,10 @@
         <v>804</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>45</v>
@@ -913,7 +1024,7 @@
         <v>364820</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
@@ -964,7 +1075,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>42</v>
@@ -973,7 +1084,7 @@
         <v>1586</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I11" s="2">
         <v>897449</v>
@@ -992,16 +1103,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2">
         <v>2741</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I12" s="2">
         <v>876960</v>
@@ -1020,7 +1131,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>43</v>
@@ -1029,7 +1140,7 @@
         <v>4443</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I13" s="2">
         <v>755050</v>
@@ -1043,12 +1154,12 @@
         <v>6620</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>44</v>
@@ -1057,7 +1168,7 @@
         <v>4047</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I14" s="2">
         <v>707650</v>
@@ -1076,7 +1187,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>45</v>
@@ -1085,7 +1196,7 @@
         <v>8968</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I15" s="2">
         <v>364820</v>
@@ -1099,7 +1210,7 @@
         <v>5991</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1152,7 +1263,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>6420</v>
+        <v>6620</v>
       </c>
       <c r="B19" s="2">
         <v>635287</v>
@@ -1160,14 +1271,20 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
       <c r="E19" s="2">
-        <v>6420</v>
+        <v>5991</v>
       </c>
       <c r="F19" s="2">
         <v>635287</v>
       </c>
       <c r="G19" s="2">
         <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>94</v>
       </c>
       <c r="N19" s="2">
         <v>4443</v>
@@ -1186,6 +1303,9 @@
       <c r="C20" s="2">
         <v>0</v>
       </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
       <c r="E20" s="2">
         <v>6620</v>
       </c>
@@ -1195,16 +1315,19 @@
       <c r="G20" s="2">
         <v>0</v>
       </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
       <c r="N20" s="2">
         <v>4047</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>5561</v>
+        <v>6620</v>
       </c>
       <c r="B21" s="2">
         <v>897449</v>
@@ -1212,8 +1335,11 @@
       <c r="C21" s="2">
         <v>2</v>
       </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
       <c r="E21" s="2">
-        <v>5561</v>
+        <v>6620</v>
       </c>
       <c r="F21" s="2">
         <v>897449</v>
@@ -1221,16 +1347,19 @@
       <c r="G21" s="2">
         <v>1</v>
       </c>
+      <c r="H21" t="s">
+        <v>95</v>
+      </c>
       <c r="N21" s="2">
         <v>8968</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>5991</v>
+        <v>6620</v>
       </c>
       <c r="B22" s="2">
         <v>876960</v>
@@ -1238,8 +1367,11 @@
       <c r="C22" s="2">
         <v>1</v>
       </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
       <c r="E22" s="2">
-        <v>5991</v>
+        <v>6620</v>
       </c>
       <c r="F22" s="2">
         <v>876960</v>
@@ -1247,10 +1379,13 @@
       <c r="G22" s="2">
         <v>2</v>
       </c>
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>3292</v>
+        <v>6620</v>
       </c>
       <c r="B23" s="2">
         <v>755050</v>
@@ -1258,14 +1393,20 @@
       <c r="C23" s="2">
         <v>0</v>
       </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
       <c r="E23" s="2">
-        <v>3292</v>
+        <v>5991</v>
       </c>
       <c r="F23" s="2">
         <v>755050</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -1278,6 +1419,9 @@
       <c r="C24" s="2">
         <v>2</v>
       </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
       <c r="E24" s="2">
         <v>6420</v>
       </c>
@@ -1287,10 +1431,13 @@
       <c r="G24" s="2">
         <v>1</v>
       </c>
+      <c r="H24" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>6620</v>
+        <v>82180</v>
       </c>
       <c r="B25" s="2">
         <v>364820</v>
@@ -1298,8 +1445,11 @@
       <c r="C25" s="2">
         <v>0</v>
       </c>
+      <c r="D25" t="s">
+        <v>88</v>
+      </c>
       <c r="E25" s="2">
-        <v>6620</v>
+        <v>5991</v>
       </c>
       <c r="F25" s="2">
         <v>364820</v>
@@ -1307,19 +1457,25 @@
       <c r="G25" s="2">
         <v>0</v>
       </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>5561</v>
+        <v>82180</v>
       </c>
       <c r="B26" s="2">
         <v>962067</v>
       </c>
       <c r="C26" s="2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>89</v>
       </c>
       <c r="E26" s="2">
-        <v>5561</v>
+        <v>5991</v>
       </c>
       <c r="F26" s="2">
         <v>962067</v>
@@ -1327,6 +1483,9 @@
       <c r="G26" s="2">
         <v>1</v>
       </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
       <c r="I26" s="3" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1495,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>5991</v>
+        <v>6420</v>
       </c>
       <c r="B27" s="2">
         <v>619043</v>
@@ -1344,6 +1503,9 @@
       <c r="C27" s="2">
         <v>1</v>
       </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
       <c r="E27" s="2">
         <v>5991</v>
       </c>
@@ -1353,6 +1515,9 @@
       <c r="G27" s="2">
         <v>0</v>
       </c>
+      <c r="H27" t="s">
+        <v>90</v>
+      </c>
       <c r="I27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1374,16 +1539,19 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>3292</v>
+        <v>5561</v>
       </c>
       <c r="B28" s="2">
-        <v>849739</v>
+        <v>619043</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
       </c>
       <c r="E28" s="2">
-        <v>3292</v>
+        <v>6420</v>
       </c>
       <c r="F28" s="2">
         <v>849739</v>
@@ -1391,8 +1559,11 @@
       <c r="G28" s="2">
         <v>2</v>
       </c>
+      <c r="H28" t="s">
+        <v>91</v>
+      </c>
       <c r="I28" s="2">
-        <v>2002</v>
+        <v>2018</v>
       </c>
       <c r="J28" s="2">
         <v>78242</v>
@@ -1400,59 +1571,80 @@
       <c r="K28" s="2">
         <v>6420</v>
       </c>
-      <c r="M28" s="2">
+      <c r="L28" t="s">
+        <v>86</v>
+      </c>
+      <c r="M28" s="6">
         <v>6420</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>49</v>
+      <c r="N28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>6420</v>
+      </c>
+      <c r="B29" s="2">
+        <v>849739</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
       <c r="I29" s="2">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="J29" s="2">
-        <v>42859</v>
+        <v>78242</v>
       </c>
       <c r="K29" s="2">
+        <v>5561</v>
+      </c>
+      <c r="L29" t="s">
+        <v>86</v>
+      </c>
+      <c r="M29" s="6">
         <v>6620</v>
       </c>
-      <c r="M29" s="2">
-        <v>6620</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>49</v>
+      <c r="N29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I30" s="2">
-        <v>2002</v>
+        <v>2018</v>
       </c>
       <c r="J30" s="2">
-        <v>78242</v>
+        <v>62098</v>
       </c>
       <c r="K30" s="2">
-        <v>5561</v>
+        <v>6620</v>
+      </c>
+      <c r="L30" t="s">
+        <v>98</v>
       </c>
       <c r="M30" s="2">
         <v>5561</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I31" s="2">
-        <v>2014</v>
+        <v>2002</v>
       </c>
       <c r="J31" s="2">
         <v>42859</v>
@@ -1460,102 +1652,155 @@
       <c r="K31" s="2">
         <v>5991</v>
       </c>
+      <c r="L31" t="s">
+        <v>46</v>
+      </c>
       <c r="M31" s="2">
         <v>5991</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I32" s="2">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="J32" s="2">
-        <v>62098</v>
+        <v>42859</v>
       </c>
       <c r="K32" s="2">
-        <v>3292</v>
+        <v>5991</v>
+      </c>
+      <c r="L32" t="s">
+        <v>46</v>
       </c>
       <c r="M32" s="2">
         <v>3292</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I33" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J33" s="2">
+        <v>82180</v>
+      </c>
+      <c r="K33" s="2">
+        <v>3292</v>
+      </c>
+      <c r="L33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I34" s="2">
+        <v>2002</v>
+      </c>
+      <c r="J34" s="2">
+        <v>62098</v>
+      </c>
+      <c r="K34" s="2">
+        <v>6620</v>
+      </c>
+      <c r="L34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I35" s="2">
+        <v>2014</v>
+      </c>
+      <c r="J35" s="2">
+        <v>62098</v>
+      </c>
+      <c r="K35" s="2">
+        <v>6620</v>
+      </c>
+      <c r="L35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I36" s="2">
+        <v>2010</v>
+      </c>
+      <c r="J36" s="2">
+        <v>62098</v>
+      </c>
+      <c r="K36" s="2">
+        <v>6620</v>
+      </c>
+      <c r="L36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I37" s="2">
+        <v>2006</v>
+      </c>
+      <c r="J37" s="2">
+        <v>62098</v>
+      </c>
+      <c r="K37" s="2">
+        <v>6620</v>
+      </c>
+      <c r="L37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I38" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>5</v>
+      <c r="F45" t="s">
+        <v>80</v>
       </c>
       <c r="N45" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>897449</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="2">
-        <v>2018</v>
-      </c>
-      <c r="F46" s="2">
-        <v>82180</v>
-      </c>
-      <c r="G46" s="2">
-        <v>2002</v>
-      </c>
-      <c r="H46" s="2">
-        <v>78242</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K46" s="1" t="s">
+      <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>0</v>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>4</v>
@@ -1566,7 +1811,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>876960</v>
+        <v>635287</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1574,25 +1819,28 @@
         <v>62</v>
       </c>
       <c r="E47" s="2">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F47" s="2">
+        <v>62098</v>
+      </c>
+      <c r="G47" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H47" s="2">
         <v>42859</v>
       </c>
-      <c r="G47" s="2">
-        <v>2006</v>
-      </c>
-      <c r="H47" s="2">
-        <v>55608</v>
-      </c>
-      <c r="J47" s="2">
-        <v>2018</v>
-      </c>
-      <c r="K47" s="2">
-        <v>82180</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>42</v>
+      <c r="I47" t="s">
+        <v>82</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="N47" s="2">
         <v>2018</v>
@@ -1603,7 +1851,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>755050</v>
+        <v>228564</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1611,36 +1859,39 @@
         <v>63</v>
       </c>
       <c r="E48" s="2">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="F48" s="2">
         <v>62098</v>
       </c>
       <c r="G48" s="2">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="H48" s="2">
         <v>82180</v>
       </c>
+      <c r="I48" t="s">
+        <v>83</v>
+      </c>
       <c r="J48" s="2">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="K48" s="2">
-        <v>42859</v>
+        <v>82180</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N48" s="2">
         <v>2014</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>707650</v>
+        <v>897449</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1648,25 +1899,28 @@
         <v>64</v>
       </c>
       <c r="E49" s="2">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="F49" s="2">
-        <v>55608</v>
+        <v>62098</v>
       </c>
       <c r="G49" s="2">
-        <v>2014</v>
-      </c>
-      <c r="H49" s="2">
+        <v>2010</v>
+      </c>
+      <c r="H49" s="5">
+        <v>78242</v>
+      </c>
+      <c r="I49" t="s">
+        <v>84</v>
+      </c>
+      <c r="J49" s="2">
+        <v>2018</v>
+      </c>
+      <c r="K49" s="2">
         <v>42859</v>
       </c>
-      <c r="J49" s="2">
-        <v>2010</v>
-      </c>
-      <c r="K49" s="2">
-        <v>62098</v>
-      </c>
       <c r="L49" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N49" s="2">
         <v>2010</v>
@@ -1677,7 +1931,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>364820</v>
+        <v>876960</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1685,25 +1939,28 @@
         <v>65</v>
       </c>
       <c r="E50" s="2">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="F50" s="2">
+        <v>62098</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2006</v>
+      </c>
+      <c r="H50" s="2">
+        <v>55608</v>
+      </c>
+      <c r="I50" t="s">
+        <v>85</v>
+      </c>
+      <c r="J50" s="2">
+        <v>2018</v>
+      </c>
+      <c r="K50" s="2">
         <v>78242</v>
       </c>
-      <c r="G50" s="2">
-        <v>2010</v>
-      </c>
-      <c r="H50" s="2">
-        <v>62098</v>
-      </c>
-      <c r="J50" s="2">
-        <v>2006</v>
-      </c>
-      <c r="K50" s="2">
-        <v>55608</v>
-      </c>
       <c r="L50" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N50" s="2">
         <v>2006</v>
@@ -1714,29 +1971,36 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>962067</v>
+        <v>755050</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E51" s="2">
+        <v>2002</v>
+      </c>
+      <c r="F51" s="2">
+        <v>62098</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H51" s="2">
+        <v>42859</v>
+      </c>
+      <c r="I51" t="s">
+        <v>82</v>
+      </c>
+      <c r="J51" s="2">
         <v>2018</v>
       </c>
-      <c r="F51" s="2">
-        <v>82180</v>
-      </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="J51" s="2">
-        <v>2002</v>
-      </c>
       <c r="K51" s="2">
-        <v>78242</v>
+        <v>55608</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N51" s="2">
         <v>2002</v>
@@ -1747,7 +2011,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>635287</v>
+        <v>707650</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1755,17 +2019,33 @@
         <v>62</v>
       </c>
       <c r="E52" s="2">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F52" s="2">
-        <v>42859</v>
-      </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+        <v>78242</v>
+      </c>
+      <c r="G52" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H52" s="2">
+        <v>55608</v>
+      </c>
+      <c r="I52" t="s">
+        <v>87</v>
+      </c>
+      <c r="J52" s="2">
+        <v>2018</v>
+      </c>
+      <c r="K52" s="2">
+        <v>62098</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>619043</v>
+        <v>364820</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1773,17 +2053,33 @@
         <v>63</v>
       </c>
       <c r="E53" s="2">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="F53" s="2">
+        <v>82180</v>
+      </c>
+      <c r="G53" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H53" s="2">
+        <v>55608</v>
+      </c>
+      <c r="I53" t="s">
+        <v>88</v>
+      </c>
+      <c r="J53" s="2">
+        <v>2014</v>
+      </c>
+      <c r="K53" s="2">
         <v>62098</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="L53" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>849739</v>
+        <v>962067</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1791,17 +2087,33 @@
         <v>64</v>
       </c>
       <c r="E54" s="2">
-        <v>2006</v>
+        <v>2018</v>
       </c>
       <c r="F54" s="2">
-        <v>55608</v>
-      </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+        <v>82180</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H54" s="2">
+        <v>62098</v>
+      </c>
+      <c r="I54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J54" s="2">
+        <v>2010</v>
+      </c>
+      <c r="K54" s="2">
+        <v>62098</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>228564</v>
+        <v>619043</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1809,13 +2121,107 @@
         <v>65</v>
       </c>
       <c r="E55" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F55" s="2">
+        <v>82180</v>
+      </c>
+      <c r="G55" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H55" s="2">
+        <v>78242</v>
+      </c>
+      <c r="I55" t="s">
+        <v>90</v>
+      </c>
+      <c r="J55" s="2">
+        <v>2006</v>
+      </c>
+      <c r="K55" s="2">
+        <v>62098</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>849739</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F56" s="2">
+        <v>78242</v>
+      </c>
+      <c r="G56" s="2">
+        <v>2018</v>
+      </c>
+      <c r="H56" s="2">
+        <v>62098</v>
+      </c>
+      <c r="I56" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="2">
         <v>2002</v>
       </c>
-      <c r="F55" s="2">
+      <c r="K56" s="2">
+        <v>62098</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J57" s="2">
+        <v>2014</v>
+      </c>
+      <c r="K57" s="2">
+        <v>82180</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J58" s="2">
+        <v>2010</v>
+      </c>
+      <c r="K58" s="5">
         <v>78242</v>
       </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="L58" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J59" s="2">
+        <v>2006</v>
+      </c>
+      <c r="K59" s="2">
+        <v>55608</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J60" s="2">
+        <v>2002</v>
+      </c>
+      <c r="K60" s="2">
+        <v>42859</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
updated date and time in match table, ordered insert queries to avoid primary key conflicts
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0654F1BA-3710-6942-A7D1-8A92DB8D2A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0ADE4C-3414-3843-BDE6-D215C35FBC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="500" windowWidth="55800" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
+    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -345,6 +345,36 @@
   </si>
   <si>
     <t>england 2006</t>
+  </si>
+  <si>
+    <t>2012-06-21</t>
+  </si>
+  <si>
+    <t>2014-07-08</t>
+  </si>
+  <si>
+    <t>2006-05-29</t>
+  </si>
+  <si>
+    <t>2010-07-21</t>
+  </si>
+  <si>
+    <t>2002-06-02</t>
+  </si>
+  <si>
+    <t>2018-08-19</t>
+  </si>
+  <si>
+    <t>2018-06-19</t>
+  </si>
+  <si>
+    <t>2018-07-04</t>
+  </si>
+  <si>
+    <t>2018-09-01</t>
+  </si>
+  <si>
+    <t>2018-04-31</t>
   </si>
 </sst>
 </file>
@@ -455,7 +485,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -464,6 +494,8 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -786,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1469,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>82180</v>
+        <v>3292</v>
       </c>
       <c r="B25" s="2">
         <v>364820</v>
@@ -1463,7 +1495,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>82180</v>
+        <v>3292</v>
       </c>
       <c r="B26" s="2">
         <v>962067</v>
@@ -1813,8 +1845,12 @@
       <c r="A47" s="2">
         <v>635287</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="9">
+        <v>0.81261574074074072</v>
+      </c>
       <c r="D47" s="2" t="s">
         <v>62</v>
       </c>
@@ -1853,8 +1889,12 @@
       <c r="A48" s="2">
         <v>228564</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D48" s="2" t="s">
         <v>63</v>
       </c>
@@ -1893,8 +1933,12 @@
       <c r="A49" s="2">
         <v>897449</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="B49" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="9">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="D49" s="2" t="s">
         <v>64</v>
       </c>
@@ -1933,8 +1977,12 @@
       <c r="A50" s="2">
         <v>876960</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.67708333333333337</v>
+      </c>
       <c r="D50" s="2" t="s">
         <v>65</v>
       </c>
@@ -1973,8 +2021,12 @@
       <c r="A51" s="2">
         <v>755050</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="9">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="D51" s="2" t="s">
         <v>66</v>
       </c>
@@ -2013,8 +2065,12 @@
       <c r="A52" s="2">
         <v>707650</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0.75694444444444453</v>
+      </c>
       <c r="D52" s="2" t="s">
         <v>62</v>
       </c>
@@ -2047,8 +2103,12 @@
       <c r="A53" s="2">
         <v>364820</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.74305555555555547</v>
+      </c>
       <c r="D53" s="2" t="s">
         <v>63</v>
       </c>
@@ -2081,8 +2141,12 @@
       <c r="A54" s="2">
         <v>962067</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0.68402777777777779</v>
+      </c>
       <c r="D54" s="2" t="s">
         <v>64</v>
       </c>
@@ -2115,8 +2179,12 @@
       <c r="A55" s="2">
         <v>619043</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="D55" s="2" t="s">
         <v>65</v>
       </c>
@@ -2149,8 +2217,12 @@
       <c r="A56" s="2">
         <v>849739</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="B56" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="9">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D56" s="2" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
all insert queries complete
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0ADE4C-3414-3843-BDE6-D215C35FBC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD88363-606B-8D49-9AD1-192F5147261F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>2018-04-31</t>
+  </si>
+  <si>
+    <t>Goalkeeper</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -496,6 +499,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -818,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,11 +1125,15 @@
       <c r="I11" s="2">
         <v>897449</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2">
+        <v>27</v>
+      </c>
       <c r="K11" s="2">
         <v>918</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="L11" s="10">
+        <v>19.989999999999998</v>
+      </c>
       <c r="N11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1149,11 +1157,15 @@
       <c r="I12" s="2">
         <v>876960</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2">
+        <v>33</v>
+      </c>
       <c r="K12" s="2">
         <v>501</v>
       </c>
-      <c r="L12" s="2"/>
+      <c r="L12" s="10">
+        <v>20</v>
+      </c>
       <c r="N12" s="2">
         <v>6420</v>
       </c>
@@ -1177,11 +1189,15 @@
       <c r="I13" s="2">
         <v>755050</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2">
+        <v>59</v>
+      </c>
       <c r="K13" s="2">
         <v>168</v>
       </c>
-      <c r="L13" s="2"/>
+      <c r="L13" s="10">
+        <v>20.010000000000002</v>
+      </c>
       <c r="N13" s="2">
         <v>6620</v>
       </c>
@@ -1205,11 +1221,15 @@
       <c r="I14" s="2">
         <v>707650</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2">
+        <v>11</v>
+      </c>
       <c r="K14" s="2">
         <v>576</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="L14" s="10">
+        <v>1000</v>
+      </c>
       <c r="N14" s="2">
         <v>5561</v>
       </c>
@@ -1233,11 +1253,15 @@
       <c r="I15" s="2">
         <v>364820</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2">
+        <v>96</v>
+      </c>
       <c r="K15" s="2">
         <v>804</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="10">
+        <v>5</v>
+      </c>
       <c r="N15" s="2">
         <v>5991</v>
       </c>
@@ -1610,7 +1634,7 @@
         <v>6420</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
changed names in member table
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD88363-606B-8D49-9AD1-192F5147261F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FEBF3E-76D8-DC47-B890-5073163434CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27140" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -378,6 +378,39 @@
   </si>
   <si>
     <t>Goalkeeper</t>
+  </si>
+  <si>
+    <t>MemberId</t>
+  </si>
+  <si>
+    <t>Aubrey Grahm</t>
+  </si>
+  <si>
+    <t>Michael Mouse</t>
+  </si>
+  <si>
+    <t>Kanye West</t>
+  </si>
+  <si>
+    <t>Kendrick Lamar</t>
+  </si>
+  <si>
+    <t>Sponge Robert</t>
+  </si>
+  <si>
+    <t>Eugene Krabs</t>
+  </si>
+  <si>
+    <t>Robert theBuilder</t>
+  </si>
+  <si>
+    <t>Zion Willaims</t>
+  </si>
+  <si>
+    <t>Tracy Mcgrady</t>
+  </si>
+  <si>
+    <t>Vince Carter</t>
   </si>
 </sst>
 </file>
@@ -822,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:G28"/>
+    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,10 +1168,10 @@
         <v>19.989999999999998</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1170,7 +1203,7 @@
         <v>6420</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1202,7 +1235,7 @@
         <v>6620</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1234,7 +1267,7 @@
         <v>5561</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1266,7 +1299,7 @@
         <v>5991</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1274,7 +1307,7 @@
         <v>3292</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -1288,7 +1321,7 @@
         <v>1586</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1314,7 +1347,7 @@
         <v>2741</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1346,7 +1379,7 @@
         <v>4443</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1378,7 +1411,7 @@
         <v>4047</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -1410,7 +1443,7 @@
         <v>8968</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added australian janitor to test data
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FEBF3E-76D8-DC47-B890-5073163434CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37D4222-B30B-2D4C-8642-92DBB08DB992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27140" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="126">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -314,9 +314,6 @@
     <t>australia+england 2018</t>
   </si>
   <si>
-    <t>table has more connections^^^</t>
-  </si>
-  <si>
     <t>england+united states 2014</t>
   </si>
   <si>
@@ -411,13 +408,19 @@
   </si>
   <si>
     <t>Vince Carter</t>
+  </si>
+  <si>
+    <t>2018 aussie janitor^^</t>
+  </si>
+  <si>
+    <t>Australian Janitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,13 +443,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -462,7 +458,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,11 +483,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -512,35 +503,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
-    <cellStyle name="Bad" xfId="4" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -855,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,11 +1152,11 @@
       <c r="K11" s="2">
         <v>918</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <v>19.989999999999998</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>1</v>
@@ -1196,14 +1184,14 @@
       <c r="K12" s="2">
         <v>501</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <v>20</v>
       </c>
       <c r="N12" s="2">
         <v>6420</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1228,14 +1216,14 @@
       <c r="K13" s="2">
         <v>168</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="9">
         <v>20.010000000000002</v>
       </c>
       <c r="N13" s="2">
         <v>6620</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1260,14 +1248,14 @@
       <c r="K14" s="2">
         <v>576</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <v>1000</v>
       </c>
       <c r="N14" s="2">
         <v>5561</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1292,28 +1280,37 @@
       <c r="K15" s="2">
         <v>804</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="9">
         <v>5</v>
       </c>
       <c r="N15" s="2">
         <v>5991</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D16" s="2">
+        <v>7420</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="N16" s="2">
         <v>3292</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="D17" t="s">
+        <v>124</v>
+      </c>
       <c r="E17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1318,7 @@
         <v>1586</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1347,7 +1344,7 @@
         <v>2741</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1373,13 +1370,13 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N19" s="2">
         <v>4443</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1405,13 +1402,13 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N20" s="2">
         <v>4047</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -1437,13 +1434,13 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N21" s="2">
         <v>8968</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -1469,7 +1466,13 @@
         <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="N22" s="2">
+        <v>7420</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -1495,7 +1498,10 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="N23" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -1667,7 +1673,7 @@
         <v>6420</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>50</v>
@@ -1719,7 +1725,7 @@
         <v>6620</v>
       </c>
       <c r="L30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M30" s="2">
         <v>5561</v>
@@ -1802,7 +1808,7 @@
         <v>6620</v>
       </c>
       <c r="L34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -1816,7 +1822,7 @@
         <v>6620</v>
       </c>
       <c r="L35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -1830,7 +1836,7 @@
         <v>6620</v>
       </c>
       <c r="L36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -1844,12 +1850,23 @@
         <v>6620</v>
       </c>
       <c r="L37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I38" s="7" t="s">
-        <v>92</v>
+      <c r="I38" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J38" s="2">
+        <v>78242</v>
+      </c>
+      <c r="K38" s="2">
+        <v>7420</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -1902,10 +1919,10 @@
       <c r="A47" s="2">
         <v>635287</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="9">
+      <c r="B47" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="8">
         <v>0.81261574074074072</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -1946,10 +1963,10 @@
       <c r="A48" s="2">
         <v>228564</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="9">
+      <c r="B48" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="8">
         <v>0.77083333333333337</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -1990,10 +2007,10 @@
       <c r="A49" s="2">
         <v>897449</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="9">
+      <c r="B49" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="8">
         <v>0.72916666666666663</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2034,10 +2051,10 @@
       <c r="A50" s="2">
         <v>876960</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="9">
+      <c r="B50" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="8">
         <v>0.67708333333333337</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2078,10 +2095,10 @@
       <c r="A51" s="2">
         <v>755050</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" s="9">
+      <c r="B51" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="8">
         <v>0.82291666666666663</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2122,10 +2139,10 @@
       <c r="A52" s="2">
         <v>707650</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="9">
+      <c r="B52" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="8">
         <v>0.75694444444444453</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2160,10 +2177,10 @@
       <c r="A53" s="2">
         <v>364820</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="9">
+      <c r="B53" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="8">
         <v>0.74305555555555547</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2198,10 +2215,10 @@
       <c r="A54" s="2">
         <v>962067</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="9">
+      <c r="B54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="8">
         <v>0.68402777777777779</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2236,10 +2253,10 @@
       <c r="A55" s="2">
         <v>619043</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="9">
+      <c r="B55" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="8">
         <v>0.89583333333333337</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -2274,10 +2291,10 @@
       <c r="A56" s="2">
         <v>849739</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="9">
+      <c r="B56" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="8">
         <v>0.77083333333333337</v>
       </c>
       <c r="D56" s="2" t="s">

</xml_diff>

<commit_message>
added minions and finished 5
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5243E4FE-7887-7342-8462-42BC9AD7F17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDB4AA2-503C-334E-8AD0-A2AEBD5BD777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27140" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -414,13 +414,31 @@
   </si>
   <si>
     <t>Australian Janitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iceland = </t>
+  </si>
+  <si>
+    <t>2018 aussie janitor ==&gt;</t>
+  </si>
+  <si>
+    <t>three new iceland</t>
+  </si>
+  <si>
+    <t>minion one</t>
+  </si>
+  <si>
+    <t>minion two</t>
+  </si>
+  <si>
+    <t>minion three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -457,8 +475,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +518,28 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -503,15 +550,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -522,12 +573,20 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
+    <cellStyle name="20% - Accent4" xfId="9" builtinId="42"/>
     <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent4" xfId="8" builtinId="41"/>
+    <cellStyle name="Good" xfId="6" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -841,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,9 +1153,6 @@
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="I9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1108,12 +1164,6 @@
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1137,12 +1187,6 @@
       <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2">
-        <v>1586</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I11" s="2">
         <v>897449</v>
       </c>
@@ -1169,12 +1213,6 @@
       <c r="B12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="2">
-        <v>2741</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="I12" s="2">
         <v>876960</v>
       </c>
@@ -1201,12 +1239,6 @@
       <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2">
-        <v>4443</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="I13" s="2">
         <v>755050</v>
       </c>
@@ -1233,12 +1265,6 @@
       <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="2">
-        <v>4047</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="I14" s="2">
         <v>707650</v>
       </c>
@@ -1265,12 +1291,6 @@
       <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="2">
-        <v>8968</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="I15" s="2">
         <v>364820</v>
       </c>
@@ -1291,12 +1311,6 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D16" s="2">
-        <v>7420</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I16" s="2">
         <v>897449</v>
       </c>
@@ -1448,10 +1462,10 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="12">
         <v>6620</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="10">
         <v>897449</v>
       </c>
       <c r="C21" s="2">
@@ -1480,10 +1494,10 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="12">
         <v>6620</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="10">
         <v>876960</v>
       </c>
       <c r="C22" s="2">
@@ -1512,10 +1526,10 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="12">
         <v>6620</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="10">
         <v>755050</v>
       </c>
       <c r="C23" s="2">
@@ -1536,15 +1550,18 @@
       <c r="H23" t="s">
         <v>96</v>
       </c>
-      <c r="N23" t="s">
-        <v>124</v>
+      <c r="N23" s="2">
+        <v>5256</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="13">
         <v>6420</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="10">
         <v>707650</v>
       </c>
       <c r="C24" s="2">
@@ -1565,12 +1582,18 @@
       <c r="H24" t="s">
         <v>87</v>
       </c>
+      <c r="N24" s="2">
+        <v>8357</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="11">
         <v>3292</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="10">
         <v>364820</v>
       </c>
       <c r="C25" s="2">
@@ -1590,6 +1613,12 @@
       </c>
       <c r="H25" t="s">
         <v>88</v>
+      </c>
+      <c r="N25" s="2">
+        <v>9463</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -1890,6 +1919,9 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>127</v>
+      </c>
       <c r="I38" s="2">
         <v>2018</v>
       </c>
@@ -1901,8 +1933,47 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I39" t="s">
-        <v>124</v>
+      <c r="I39" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J39" s="2">
+        <v>42859</v>
+      </c>
+      <c r="K39" s="2">
+        <v>5256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I40" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J40" s="2">
+        <v>42859</v>
+      </c>
+      <c r="K40" s="2">
+        <v>8357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2018</v>
+      </c>
+      <c r="J41" s="2">
+        <v>42859</v>
+      </c>
+      <c r="K41" s="2">
+        <v>9463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="2">
+        <v>42859</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2395,6 +2466,9 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="J60" s="2">
         <v>2002</v>
       </c>
@@ -2403,6 +2477,86 @@
       </c>
       <c r="L60" s="2" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>1586</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>2741</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>4443</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>4047</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>8968</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>7420</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>5256</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>8357</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>9463</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2414,5 +2568,6 @@
     <hyperlink ref="F7" r:id="rId5" xr:uid="{7C1C7E9F-593E-D349-9489-DC2EA7F0DA6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
formatted nicely, only need question 3 now
</commit_message>
<xml_diff>
--- a/WorldCupSampleData.xlsx
+++ b/WorldCupSampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Desktop/WorldCupRepo/WorldCupDataBaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDB4AA2-503C-334E-8AD0-A2AEBD5BD777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A6580-7F9E-DF43-9F51-D63F24A357E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="32180" xr2:uid="{169D28DA-BAA8-6B4F-9A73-6592D4D8237F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>iceland</t>
-  </si>
-  <si>
     <t>Iceland</t>
   </si>
   <si>
@@ -281,69 +278,6 @@
     <t>all england</t>
   </si>
   <si>
-    <t>united states</t>
-  </si>
-  <si>
-    <t>england+iceland</t>
-  </si>
-  <si>
-    <t>england+united states</t>
-  </si>
-  <si>
-    <t>england+australia</t>
-  </si>
-  <si>
-    <t>england+germany</t>
-  </si>
-  <si>
-    <t>australian</t>
-  </si>
-  <si>
-    <t>australia+germany 2018</t>
-  </si>
-  <si>
-    <t>united states+germany 2018</t>
-  </si>
-  <si>
-    <t>united states+england 2018</t>
-  </si>
-  <si>
-    <t>united states+australia 2018</t>
-  </si>
-  <si>
-    <t>australia+england 2018</t>
-  </si>
-  <si>
-    <t>england+united states 2014</t>
-  </si>
-  <si>
-    <t>england+iceland 2018</t>
-  </si>
-  <si>
-    <t>england+australia 2010</t>
-  </si>
-  <si>
-    <t>england+germany 2006</t>
-  </si>
-  <si>
-    <t>england+iceland 2002</t>
-  </si>
-  <si>
-    <t>england 2018</t>
-  </si>
-  <si>
-    <t>england 2002</t>
-  </si>
-  <si>
-    <t>england 2014</t>
-  </si>
-  <si>
-    <t>england 2010</t>
-  </si>
-  <si>
-    <t>england 2006</t>
-  </si>
-  <si>
     <t>2012-06-21</t>
   </si>
   <si>
@@ -410,19 +344,7 @@
     <t>Vince Carter</t>
   </si>
   <si>
-    <t>2018 aussie janitor^^</t>
-  </si>
-  <si>
     <t>Australian Janitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iceland = </t>
-  </si>
-  <si>
-    <t>2018 aussie janitor ==&gt;</t>
-  </si>
-  <si>
-    <t>three new iceland</t>
   </si>
   <si>
     <t>minion one</t>
@@ -438,7 +360,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -475,15 +397,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,35 +423,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9E1F2"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -550,44 +443,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
-    <cellStyle name="20% - Accent4" xfId="9" builtinId="42"/>
-    <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
-    <cellStyle name="Accent4" xfId="8" builtinId="41"/>
-    <cellStyle name="Good" xfId="6" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -902,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3241CF3D-FE43-164D-87A5-0650F94797C5}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23:O25"/>
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,10 +866,10 @@
         <v>918</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>42</v>
@@ -1000,7 +881,7 @@
         <v>897449</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M3" s="2">
         <v>1</v>
@@ -1011,7 +892,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2">
         <v>372295</v>
@@ -1020,13 +901,13 @@
         <v>501</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="2">
         <v>635287</v>
@@ -1035,7 +916,7 @@
         <v>876960</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
@@ -1055,10 +936,10 @@
         <v>168</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>43</v>
@@ -1070,7 +951,7 @@
         <v>755050</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M5" s="2">
         <v>2</v>
@@ -1090,10 +971,10 @@
         <v>576</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>44</v>
@@ -1105,7 +986,7 @@
         <v>707650</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M6" s="2">
         <v>0</v>
@@ -1125,10 +1006,10 @@
         <v>804</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>45</v>
@@ -1140,7 +1021,7 @@
         <v>364820</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
@@ -1182,7 +1063,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>42</v>
@@ -1196,11 +1077,11 @@
       <c r="K11" s="2">
         <v>918</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="8">
         <v>19.989999999999998</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>1</v>
@@ -1208,10 +1089,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="2">
         <v>876960</v>
@@ -1222,19 +1103,19 @@
       <c r="K12" s="2">
         <v>501</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="8">
         <v>20</v>
       </c>
       <c r="N12" s="2">
         <v>6420</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>43</v>
@@ -1248,19 +1129,19 @@
       <c r="K13" s="2">
         <v>168</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <v>20.010000000000002</v>
       </c>
       <c r="N13" s="2">
         <v>6620</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>44</v>
@@ -1274,19 +1155,19 @@
       <c r="K14" s="2">
         <v>576</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>1000</v>
       </c>
       <c r="N14" s="2">
         <v>5561</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>45</v>
@@ -1300,14 +1181,14 @@
       <c r="K15" s="2">
         <v>804</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="8">
         <v>5</v>
       </c>
       <c r="N15" s="2">
         <v>5991</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1320,23 +1201,20 @@
       <c r="K16" s="2">
         <v>918</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="8">
         <v>19.989999999999998</v>
       </c>
       <c r="N16" s="2">
         <v>3292</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
-        <v>124</v>
-      </c>
       <c r="E17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1349,14 +1227,14 @@
       <c r="K17" s="2">
         <v>918</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="8">
         <v>19.989999999999998</v>
       </c>
       <c r="N17" s="2">
         <v>1586</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1387,14 +1265,14 @@
       <c r="K18" s="2">
         <v>576</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="8">
         <v>1000</v>
       </c>
       <c r="N18" s="2">
         <v>2741</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1407,9 +1285,6 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
       <c r="E19" s="2">
         <v>5991</v>
       </c>
@@ -1419,14 +1294,11 @@
       <c r="G19" s="2">
         <v>3</v>
       </c>
-      <c r="H19" t="s">
-        <v>93</v>
-      </c>
       <c r="N19" s="2">
         <v>4443</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1437,10 +1309,7 @@
         <v>228564</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2">
         <v>6620</v>
@@ -1449,31 +1318,25 @@
         <v>228564</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="N20" s="2">
         <v>4047</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="12">
+      <c r="A21" s="9">
         <v>6620</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>897449</v>
       </c>
       <c r="C21" s="2">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
       <c r="E21" s="2">
         <v>6620</v>
       </c>
@@ -1483,29 +1346,23 @@
       <c r="G21" s="2">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
-        <v>94</v>
-      </c>
       <c r="N21" s="2">
         <v>8968</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
+      <c r="A22" s="9">
         <v>6620</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>876960</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
       <c r="E22" s="2">
         <v>6620</v>
       </c>
@@ -1515,28 +1372,22 @@
       <c r="G22" s="2">
         <v>2</v>
       </c>
-      <c r="H22" t="s">
-        <v>95</v>
-      </c>
       <c r="N22" s="2">
         <v>7420</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
+      <c r="A23" s="9">
         <v>6620</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>755050</v>
       </c>
       <c r="C23" s="2">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="E23" s="2">
         <v>5991</v>
@@ -1545,31 +1396,25 @@
         <v>755050</v>
       </c>
       <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="N23" s="2">
         <v>5256</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+      <c r="A24" s="9">
         <v>6420</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>707650</v>
       </c>
       <c r="C24" s="2">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
-        <v>87</v>
-      </c>
       <c r="E24" s="2">
         <v>6420</v>
       </c>
@@ -1579,28 +1424,22 @@
       <c r="G24" s="2">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
-        <v>87</v>
-      </c>
       <c r="N24" s="2">
         <v>8357</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
+      <c r="A25" s="9">
         <v>3292</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>364820</v>
       </c>
       <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="E25" s="2">
         <v>5991</v>
@@ -1609,16 +1448,13 @@
         <v>364820</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="N25" s="2">
         <v>9463</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -1631,9 +1467,6 @@
       <c r="C26" s="2">
         <v>2</v>
       </c>
-      <c r="D26" t="s">
-        <v>89</v>
-      </c>
       <c r="E26" s="2">
         <v>5991</v>
       </c>
@@ -1642,9 +1475,6 @@
       </c>
       <c r="G26" s="2">
         <v>1</v>
-      </c>
-      <c r="H26" t="s">
-        <v>89</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>14</v>
@@ -1663,9 +1493,6 @@
       <c r="C27" s="2">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
       <c r="E27" s="2">
         <v>5991</v>
       </c>
@@ -1673,10 +1500,7 @@
         <v>619043</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>4</v>
@@ -1707,9 +1531,6 @@
       <c r="C28" s="2">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
-        <v>90</v>
-      </c>
       <c r="E28" s="2">
         <v>6420</v>
       </c>
@@ -1719,9 +1540,6 @@
       <c r="G28" s="2">
         <v>2</v>
       </c>
-      <c r="H28" t="s">
-        <v>91</v>
-      </c>
       <c r="I28" s="2">
         <v>2018</v>
       </c>
@@ -1731,17 +1549,14 @@
       <c r="K28" s="2">
         <v>6420</v>
       </c>
-      <c r="L28" t="s">
-        <v>86</v>
-      </c>
-      <c r="M28" s="6">
+      <c r="M28" s="9">
         <v>6420</v>
       </c>
-      <c r="N28" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>50</v>
+      <c r="N28" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="O28" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -1752,10 +1567,7 @@
         <v>849739</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="I29" s="2">
         <v>2018</v>
@@ -1766,17 +1578,14 @@
       <c r="K29" s="2">
         <v>5561</v>
       </c>
-      <c r="L29" t="s">
-        <v>86</v>
-      </c>
-      <c r="M29" s="6">
+      <c r="M29" s="9">
         <v>6620</v>
       </c>
-      <c r="N29" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>50</v>
+      <c r="N29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="O29" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -1789,17 +1598,14 @@
       <c r="K30" s="2">
         <v>6620</v>
       </c>
-      <c r="L30" t="s">
-        <v>97</v>
-      </c>
       <c r="M30" s="2">
         <v>5561</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -1812,17 +1618,14 @@
       <c r="K31" s="2">
         <v>5991</v>
       </c>
-      <c r="L31" t="s">
-        <v>46</v>
-      </c>
       <c r="M31" s="2">
         <v>5991</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -1835,17 +1638,14 @@
       <c r="K32" s="2">
         <v>5991</v>
       </c>
-      <c r="L32" t="s">
-        <v>46</v>
-      </c>
       <c r="M32" s="2">
         <v>3292</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -1857,9 +1657,6 @@
       </c>
       <c r="K33" s="2">
         <v>3292</v>
-      </c>
-      <c r="L33" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -1872,9 +1669,6 @@
       <c r="K34" s="2">
         <v>6620</v>
       </c>
-      <c r="L34" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I35" s="2">
@@ -1886,9 +1680,6 @@
       <c r="K35" s="2">
         <v>6620</v>
       </c>
-      <c r="L35" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I36" s="2">
@@ -1900,9 +1691,6 @@
       <c r="K36" s="2">
         <v>6620</v>
       </c>
-      <c r="L36" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I37" s="2">
@@ -1914,14 +1702,8 @@
       <c r="K37" s="2">
         <v>6620</v>
       </c>
-      <c r="L37" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H38" t="s">
-        <v>127</v>
-      </c>
       <c r="I38" s="2">
         <v>2018</v>
       </c>
@@ -1955,9 +1737,6 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H41" t="s">
-        <v>128</v>
-      </c>
       <c r="I41" s="2">
         <v>2018</v>
       </c>
@@ -1966,14 +1745,6 @@
       </c>
       <c r="K41" s="2">
         <v>9463</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="2">
-        <v>42859</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -1981,7 +1752,7 @@
         <v>17</v>
       </c>
       <c r="F45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N45" s="3" t="s">
         <v>3</v>
@@ -2026,14 +1797,14 @@
       <c r="A47" s="2">
         <v>635287</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="8">
+      <c r="B47" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="7">
         <v>0.81261574074074072</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" s="2">
         <v>2018</v>
@@ -2046,9 +1817,6 @@
       </c>
       <c r="H47" s="2">
         <v>42859</v>
-      </c>
-      <c r="I47" t="s">
-        <v>82</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>4</v>
@@ -2070,14 +1838,14 @@
       <c r="A48" s="2">
         <v>228564</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="8">
+      <c r="B48" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48" s="2">
         <v>2014</v>
@@ -2091,9 +1859,6 @@
       <c r="H48" s="2">
         <v>82180</v>
       </c>
-      <c r="I48" t="s">
-        <v>83</v>
-      </c>
       <c r="J48" s="2">
         <v>2018</v>
       </c>
@@ -2107,21 +1872,21 @@
         <v>2014</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>897449</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="8">
+      <c r="B49" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="7">
         <v>0.72916666666666663</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E49" s="2">
         <v>2010</v>
@@ -2135,9 +1900,6 @@
       <c r="H49" s="5">
         <v>78242</v>
       </c>
-      <c r="I49" t="s">
-        <v>84</v>
-      </c>
       <c r="J49" s="2">
         <v>2018</v>
       </c>
@@ -2145,7 +1907,7 @@
         <v>42859</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N49" s="2">
         <v>2010</v>
@@ -2158,14 +1920,14 @@
       <c r="A50" s="2">
         <v>876960</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="8">
+      <c r="B50" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="7">
         <v>0.67708333333333337</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E50" s="2">
         <v>2006</v>
@@ -2178,9 +1940,6 @@
       </c>
       <c r="H50" s="2">
         <v>55608</v>
-      </c>
-      <c r="I50" t="s">
-        <v>85</v>
       </c>
       <c r="J50" s="2">
         <v>2018</v>
@@ -2202,14 +1961,14 @@
       <c r="A51" s="2">
         <v>755050</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="8">
+      <c r="B51" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="7">
         <v>0.82291666666666663</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="2">
         <v>2002</v>
@@ -2222,9 +1981,6 @@
       </c>
       <c r="H51" s="2">
         <v>42859</v>
-      </c>
-      <c r="I51" t="s">
-        <v>82</v>
       </c>
       <c r="J51" s="2">
         <v>2018</v>
@@ -2246,14 +2002,14 @@
       <c r="A52" s="2">
         <v>707650</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="8">
+      <c r="B52" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="7">
         <v>0.75694444444444453</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E52" s="2">
         <v>2018</v>
@@ -2266,9 +2022,6 @@
       </c>
       <c r="H52" s="2">
         <v>55608</v>
-      </c>
-      <c r="I52" t="s">
-        <v>87</v>
       </c>
       <c r="J52" s="2">
         <v>2018</v>
@@ -2284,14 +2037,14 @@
       <c r="A53" s="2">
         <v>364820</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="8">
+      <c r="B53" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="7">
         <v>0.74305555555555547</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E53" s="2">
         <v>2018</v>
@@ -2304,9 +2057,6 @@
       </c>
       <c r="H53" s="2">
         <v>55608</v>
-      </c>
-      <c r="I53" t="s">
-        <v>88</v>
       </c>
       <c r="J53" s="2">
         <v>2014</v>
@@ -2322,14 +2072,14 @@
       <c r="A54" s="2">
         <v>962067</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="8">
+      <c r="B54" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="7">
         <v>0.68402777777777779</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E54" s="2">
         <v>2018</v>
@@ -2342,9 +2092,6 @@
       </c>
       <c r="H54" s="2">
         <v>62098</v>
-      </c>
-      <c r="I54" t="s">
-        <v>89</v>
       </c>
       <c r="J54" s="2">
         <v>2010</v>
@@ -2360,14 +2107,14 @@
       <c r="A55" s="2">
         <v>619043</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C55" s="8">
+      <c r="B55" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="7">
         <v>0.89583333333333337</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E55" s="2">
         <v>2018</v>
@@ -2380,9 +2127,6 @@
       </c>
       <c r="H55" s="2">
         <v>78242</v>
-      </c>
-      <c r="I55" t="s">
-        <v>90</v>
       </c>
       <c r="J55" s="2">
         <v>2006</v>
@@ -2398,14 +2142,14 @@
       <c r="A56" s="2">
         <v>849739</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="8">
+      <c r="B56" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="7">
         <v>0.77083333333333337</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E56" s="2">
         <v>2018</v>
@@ -2418,9 +2162,6 @@
       </c>
       <c r="H56" s="2">
         <v>62098</v>
-      </c>
-      <c r="I56" t="s">
-        <v>91</v>
       </c>
       <c r="J56" s="2">
         <v>2002</v>
@@ -2476,7 +2217,7 @@
         <v>42859</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
@@ -2492,7 +2233,7 @@
         <v>1586</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -2500,7 +2241,7 @@
         <v>2741</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -2508,7 +2249,7 @@
         <v>4443</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2516,7 +2257,7 @@
         <v>4047</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2524,7 +2265,7 @@
         <v>8968</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2532,7 +2273,7 @@
         <v>7420</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2540,7 +2281,7 @@
         <v>5256</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -2548,7 +2289,7 @@
         <v>8357</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -2556,7 +2297,7 @@
         <v>9463</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>